<commit_message>
Add: Part One Code
</commit_message>
<xml_diff>
--- a/data/BCWeeklyDataMarketing.xlsx
+++ b/data/BCWeeklyDataMarketing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simoc\Desktop\Portfolio\WeRoadTHT\PartOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simoc\Desktop\Portfolio\WeRoadTHT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6AFADE-AD40-4257-B057-0D252AA6C1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EB581E-6CA5-4E34-B015-5D422A91F209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -862,7 +862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10050,13 +10052,13 @@
         <f>48073+909</f>
         <v>48982</v>
       </c>
-      <c r="M105" s="6" t="e">
-        <f>38447.66-K105-#REF!-#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N105" s="10" t="e">
-        <f>95463-L105-#REF!</f>
-        <v>#REF!</v>
+      <c r="M105" s="6">
+        <f>38447.66-K105-0-0</f>
+        <v>35032.310000000005</v>
+      </c>
+      <c r="N105" s="10">
+        <f>95463-L105-0</f>
+        <v>46481</v>
       </c>
       <c r="O105" s="6">
         <f>34720.76-R105</f>

</xml_diff>